<commit_message>
carga nueva de codigo (probablemente inestable)
</commit_message>
<xml_diff>
--- a/FACTURAS/2904001355097/FE_202009.xlsx
+++ b/FACTURAS/2904001355097/FE_202009.xlsx
@@ -1,619 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
-  </bookViews>
-  <sheets>
-    <sheet name="fe_202009" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="144525" forceFullCalc="1"/>
-</workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="199">
-  <si>
-    <t>Factura</t>
-  </si>
-  <si>
-    <t>Fecha de emisión de la factura</t>
-  </si>
-  <si>
-    <t>Número de Factura</t>
-  </si>
-  <si>
-    <t>Nombre / Nombre de compañía</t>
-  </si>
-  <si>
-    <t>Producto / Servicio</t>
-  </si>
-  <si>
-    <t>Tipo de factura</t>
-  </si>
-  <si>
-    <t>Status de Pago</t>
-  </si>
-  <si>
-    <t>Fecha de vencimiento</t>
-  </si>
-  <si>
-    <t>Moneda</t>
-  </si>
-  <si>
-    <t>Tipo de cambio</t>
-  </si>
-  <si>
-    <t>Cantidad total</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>Campos personalizados del producto</t>
-  </si>
-  <si>
-    <t>Campos personalizados del cliente</t>
-  </si>
-  <si>
-    <t>INV_1378</t>
-  </si>
-  <si>
-    <t>2020-09-02</t>
-  </si>
-  <si>
-    <t>771-0f673c43-edfa-4774-b6d7-177851828f3a</t>
-  </si>
-  <si>
-    <t>VENTURA</t>
-  </si>
-  <si>
-    <t>PAGO ANUAL DE JUNIO 2020 A MAYO 2021 (otro)</t>
-  </si>
-  <si>
-    <t>Facturado</t>
-  </si>
-  <si>
-    <t>No pagado</t>
-  </si>
-  <si>
-    <t>2020-09-07</t>
-  </si>
-  <si>
-    <t>BS</t>
-  </si>
-  <si>
-    <t>3360.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1132 - EDIFICIO: VENTURA R - 101:CODIGO CLIENTE: 1132 - EDIFICIO: VENTURA</t>
-  </si>
-  <si>
-    <t>INV_1357</t>
-  </si>
-  <si>
-    <t>769-f11cdb25-b003-460e-9c2d-652a104fc108</t>
-  </si>
-  <si>
-    <t>PENIEL</t>
-  </si>
-  <si>
-    <t>Servicio de Mantenimiento Agosto 2020 (otro)</t>
-  </si>
-  <si>
-    <t>2020-09-03</t>
-  </si>
-  <si>
-    <t>700.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 10027 - EDIFICIO: PENIEL R - 101:CODIGO CLIENTE: 10027 - EDIFICIO: PENIEL</t>
-  </si>
-  <si>
-    <t>INV_1356</t>
-  </si>
-  <si>
-    <t>770-7e52e8ea-c4e1-443b-923c-1e39944ddbaa</t>
-  </si>
-  <si>
-    <t>Servicio de Mantenimiento Julio 2020 (otro)</t>
-  </si>
-  <si>
-    <t>INV_1355</t>
-  </si>
-  <si>
-    <t>768-993aa6ee-19fa-4371-b325-c8583cedac58</t>
-  </si>
-  <si>
-    <t>TORRE ALFA</t>
-  </si>
-  <si>
-    <t>2020-09-20</t>
-  </si>
-  <si>
-    <t>610.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE 1407: EDIFICIO TORRE ALFA R - 101:CODIGO CLIENTE 1407: EDIFICIO TORRE ALFA</t>
-  </si>
-  <si>
-    <t>INV_1353</t>
-  </si>
-  <si>
-    <t>767-36062a84-6113-4f7a-b21d-0ea39fffcbdc</t>
-  </si>
-  <si>
-    <t>PALMAS</t>
-  </si>
-  <si>
-    <t>Panel de Control (pza), Lector de Tarjeta RFID de corto alcance (pza), Expansora de Pisos para control de Ascensores (pza), Servicio de Mano de Obra (otro)</t>
-  </si>
-  <si>
-    <t>2020-09-30</t>
-  </si>
-  <si>
-    <t>9486.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE : 1013 - EDIFICIO LAS PALMAS R-101:CODIGO CLIENTE : 1013 - EDIFICIO LAS PALMAS</t>
-  </si>
-  <si>
-    <t>INV_1352</t>
-  </si>
-  <si>
-    <t>766-62d0476a-f601-4df9-987e-c38193ac93b2</t>
-  </si>
-  <si>
-    <t>OPHIR</t>
-  </si>
-  <si>
-    <t>1300.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1585 - EDIFICIO: OPHIR R - 101:CODIGO CLIENTE: 1585 - EDIFICIO: OPHIR</t>
-  </si>
-  <si>
-    <t>INV_1351</t>
-  </si>
-  <si>
-    <t>765-4bb79552-c30c-4566-919d-d70c7e0006d2</t>
-  </si>
-  <si>
-    <t>Tarjeta Magnética (pza)</t>
-  </si>
-  <si>
-    <t>1800.000 Bs.</t>
-  </si>
-  <si>
-    <t>INV_1350</t>
-  </si>
-  <si>
-    <t>764-fe793491-3576-43de-90b0-dcef51ac8e1f</t>
-  </si>
-  <si>
-    <t>MONTERREY</t>
-  </si>
-  <si>
-    <t>1000.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 1433 - EDIFICIO MONTERREY R-101:CODIGO CLIENTE: 1433 - EDIFICIO MONTERREY</t>
-  </si>
-  <si>
-    <t>INV_1348</t>
-  </si>
-  <si>
-    <t>763-ad7e5801-9d55-49fa-90ae-5342a609ffa1</t>
-  </si>
-  <si>
-    <t>MAGLIA</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1579 - EDIFICIO: MAGLIA R - 101:CODIGO CLIENTE: 1579 - EDIFICIO: MAGLIA</t>
-  </si>
-  <si>
-    <t>INV_1346</t>
-  </si>
-  <si>
-    <t>762-c9c8d6ca-c9e0-44f6-b444-3b1219259f5c</t>
-  </si>
-  <si>
-    <t>INV_1344</t>
-  </si>
-  <si>
-    <t>761-9642cc9f-51dd-477f-8987-0c6cc39142a7</t>
-  </si>
-  <si>
-    <t>CRISTINA</t>
-  </si>
-  <si>
-    <t>2020-09-05</t>
-  </si>
-  <si>
-    <t>560.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1763 - EDIFICIO: CRISTINA R - 101:CODIGO CLIENTE: 1763 - EDIFICIO: CRISTINA</t>
-  </si>
-  <si>
-    <t>INV_1308</t>
-  </si>
-  <si>
-    <t>758-e933f46b-727e-402b-aeeb-357bcbfd40b4</t>
-  </si>
-  <si>
-    <t>INV_1300</t>
-  </si>
-  <si>
-    <t>755-911f8c8e-6137-4bac-8af1-0d3531269e11</t>
-  </si>
-  <si>
-    <t>VENECIA</t>
-  </si>
-  <si>
-    <t>2020-10-02</t>
-  </si>
-  <si>
-    <t>1528.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE : 1394 - EDIFICIO VENECIA R-101:CODIGO CLIENTE : 1394 - EDIFICIO VENECIA</t>
-  </si>
-  <si>
-    <t>INV_1296</t>
-  </si>
-  <si>
-    <t>2020-09-01</t>
-  </si>
-  <si>
-    <t>753-06be9cd4-6590-47a3-b080-19a078a502fb</t>
-  </si>
-  <si>
-    <t>INV_1278</t>
-  </si>
-  <si>
-    <t>751-62c04eaa-e7ef-4f69-af68-e6a22648fad7</t>
-  </si>
-  <si>
-    <t>EL FARO</t>
-  </si>
-  <si>
-    <t>2020-09-10</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 4019 - EDIFICIO: EL FARO R-101:CODIGO CLIENTE: 4019 - EDIFICIO: EL FARO</t>
-  </si>
-  <si>
-    <t>INV_1277</t>
-  </si>
-  <si>
-    <t>748-55ccd56e-5751-4f64-8068-4d1a7e0de994</t>
-  </si>
-  <si>
-    <t>MILENIO</t>
-  </si>
-  <si>
-    <t>400.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE :1197 - EDIFICIO MILENIO R-101:CODIGO CLIENTE :1197 - EDIFICIO MILENIO</t>
-  </si>
-  <si>
-    <t>INV_1276</t>
-  </si>
-  <si>
-    <t>745-ebc63717-eb75-44a0-9585-3edc44f71986</t>
-  </si>
-  <si>
-    <t>TES BIENESTAR</t>
-  </si>
-  <si>
-    <t>550.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE : 10187 - TES BIENESTAR R-101:CODIGO CLIENTE : 10187 - TES BIENESTAR</t>
-  </si>
-  <si>
-    <t>INV_1275</t>
-  </si>
-  <si>
-    <t>741-bb2aea40-bbd3-400d-a35e-9d0dad909748</t>
-  </si>
-  <si>
-    <t>SOL Y LUNA</t>
-  </si>
-  <si>
-    <t>2020-09-04</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1375 - EDIFICIO: SOL Y LUNA R - 101:CODIGO CLIENTE: 1375 - EDIFICIO: SOL Y LUNA</t>
-  </si>
-  <si>
-    <t>INV_1274</t>
-  </si>
-  <si>
-    <t>740-5f9fc3d9-6eb1-4677-a039-f4c76c23ecaf</t>
-  </si>
-  <si>
-    <t>INV_1273</t>
-  </si>
-  <si>
-    <t>739-f01a243c-6372-4166-8ce2-78a689f5e6b4</t>
-  </si>
-  <si>
-    <t>COMPANEX</t>
-  </si>
-  <si>
-    <t>720.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 1412 - EDIFICIO: COMPANEX R-101:CODIGO CLIENTE: 1412 - EDIFICIO: COMPANEX</t>
-  </si>
-  <si>
-    <t>INV_1272</t>
-  </si>
-  <si>
-    <t>738-9e8e954d-9c91-42b4-a688-b8b6d7ed1ddf</t>
-  </si>
-  <si>
-    <t>NAPOLIS</t>
-  </si>
-  <si>
-    <t>410.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE : _ 1202 - EDIFICIO : NAPOLIS R - 101:CODIGO CLIENTE : _ 1202 - EDIFICIO : NAPOLIS</t>
-  </si>
-  <si>
-    <t>INV_1271</t>
-  </si>
-  <si>
-    <t>737-062ec529-c22a-4b5d-ab6e-927274f2458a</t>
-  </si>
-  <si>
-    <t>CONDOMINIO CLAVELES DEL SUR 2da TERRAZA</t>
-  </si>
-  <si>
-    <t>5130.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1988 - EDIFICIO: CONDOMINIO CLAVELES DEL SUR 2da TERRAZA R - 101:CODIGO CLIENTE: 1988 - EDIFICIO: CONDOMINIO CLAVELES DEL SUR 2da TERRAZA</t>
-  </si>
-  <si>
-    <t>INV_1270</t>
-  </si>
-  <si>
-    <t>736-e3ce115b-4f47-47d5-b3af-1d4b685d9144</t>
-  </si>
-  <si>
-    <t>EBENEZER</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1521 - EDIFICIO: EBENEZER R - 101:CODIGO CLIENTE: 1521 - EDIFICIO: EBENEZER</t>
-  </si>
-  <si>
-    <t>INV_1269</t>
-  </si>
-  <si>
-    <t>735-8210d0ca-15ae-4142-841c-4b4b586ba71d</t>
-  </si>
-  <si>
-    <t>PORTO DI BARI</t>
-  </si>
-  <si>
-    <t>600.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1558 - EDIFICIO: PORTO DI BARI R - 101:CODIGO CLIENTE: 1558 - EDIFICIO: PORTO DI BARI</t>
-  </si>
-  <si>
-    <t>INV_1268</t>
-  </si>
-  <si>
-    <t>734-1ade37b8-0209-4453-98d6-ad85383106af</t>
-  </si>
-  <si>
-    <t>COSMOS</t>
-  </si>
-  <si>
-    <t>660.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE: 1602 - EDIFICIO: COSMOS R - 101:CODIGO CLIENTE: 1602 - EDIFICIO: COSMOS</t>
-  </si>
-  <si>
-    <t>INV_1267</t>
-  </si>
-  <si>
-    <t>733-c5e9a0ba-6775-47b5-bc13-d2cde2e321cb</t>
-  </si>
-  <si>
-    <t>INV_1265</t>
-  </si>
-  <si>
-    <t>732-8939620e-edea-48a4-8543-2861056a8909</t>
-  </si>
-  <si>
-    <t>MERAPA MICHELLINE</t>
-  </si>
-  <si>
-    <t>500.000 Bs.</t>
-  </si>
-  <si>
-    <t>R - 100:CODIGO CLIENTE : _ 1877 - EDIFICIO : _ MERAPA MICHELLINE R - 101:CODIGO CLIENTE : _ 1877 - EDIFICIO : _ MERAPA MICHELLINE</t>
-  </si>
-  <si>
-    <t>INV_1264</t>
-  </si>
-  <si>
-    <t>731-231dc340-5fa7-4ee2-ae8d-4a79b7f25ea8</t>
-  </si>
-  <si>
-    <t>INV_1261</t>
-  </si>
-  <si>
-    <t>730-72920654-c4fb-4763-89c0-b2255d3e6fbd</t>
-  </si>
-  <si>
-    <t>OBRAJES -SUR</t>
-  </si>
-  <si>
-    <t>Provisión/Instalación de Repuestos (otro)</t>
-  </si>
-  <si>
-    <t>1200.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE :1238 - TORRE OBRAJES -SUR R-101:CODIGO CLIENTE :1238 - TORRE OBRAJES -SUR</t>
-  </si>
-  <si>
-    <t>INV_1260</t>
-  </si>
-  <si>
-    <t>729-88259f3e-312c-4d6e-a177-c41e9d8f0db7</t>
-  </si>
-  <si>
-    <t>DELCAS</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 1803 EDIFICIO DELCAS R-101:CODIGO CLIENTE: 1803 EDIFICIO DELCAS</t>
-  </si>
-  <si>
-    <t>INV_1171</t>
-  </si>
-  <si>
-    <t>754-7366da64-dea4-401f-a5d9-65bb9cf6ce98</t>
-  </si>
-  <si>
-    <t>YPFB TRANSIERRA S.A.</t>
-  </si>
-  <si>
-    <t>R-100 /:Código Cliente: 2076 / Edificio: Transierra R-101 /:Código Cliente: 2076 / Edificio: Transierra</t>
-  </si>
-  <si>
-    <t>INV_1134</t>
-  </si>
-  <si>
-    <t>750-1dd2d857-14c0-4ee1-a4c8-ac987525b1b5</t>
-  </si>
-  <si>
-    <t>INV_1102</t>
-  </si>
-  <si>
-    <t>746-255e9d95-d3de-4841-883b-6c637303518e</t>
-  </si>
-  <si>
-    <t>WALTER CONDORI</t>
-  </si>
-  <si>
-    <t>R-100 /:Codigo Cliente: 2095 / Nombre del Edificio: WALTER CONDORI R-101 /:Codigo Cliente: 2095 / Nombre del Edificio: WALTER CONDORI</t>
-  </si>
-  <si>
-    <t>INV_1101</t>
-  </si>
-  <si>
-    <t>747-2e5863ab-e377-4338-8132-07f3c3b89f5e</t>
-  </si>
-  <si>
-    <t>JULIANA LARICO</t>
-  </si>
-  <si>
-    <t>R-100 /:Codigo Cliente: 2340 / Nombre del Edificio: JULIANA LARICO R-101 /:Codigo Cliente: 2340 / Nombre del Edificio: JULIANA LARICO</t>
-  </si>
-  <si>
-    <t>INV_1085</t>
-  </si>
-  <si>
-    <t>744-14652e6c-004e-417d-bafb-d6dd7ace1f14</t>
-  </si>
-  <si>
-    <t>CAJA PETROLERA DE SALUD</t>
-  </si>
-  <si>
-    <t>2020-09-25</t>
-  </si>
-  <si>
-    <t>2569.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 3100 - EDIF: CAJA PETROLERA DE SALUD R-101:CODIGO CLIENTE: 3100 - EDIF: CAJA PETROLERA DE SALUD</t>
-  </si>
-  <si>
-    <t>INV_1057</t>
-  </si>
-  <si>
-    <t>749-bc7147db-be23-4047-9e63-c4cc82bfe8db</t>
-  </si>
-  <si>
-    <t>Servicio de Mantenimiento Junio 2020 (otro)</t>
-  </si>
-  <si>
-    <t>INV_1053</t>
-  </si>
-  <si>
-    <t>757-7693fd48-4b33-4e13-b1ce-39bb35ad2b5e</t>
-  </si>
-  <si>
-    <t>CONDOMINIO RECOLETA</t>
-  </si>
-  <si>
-    <t>2020-09-24</t>
-  </si>
-  <si>
-    <t>1995.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 3055 - EDIF: CONDOMINIO RECOLETA R-101:CODIGO CLIENTE: 3055 - EDIF: CONDOMINIO RECOLETA</t>
-  </si>
-  <si>
-    <t>INV_939</t>
-  </si>
-  <si>
-    <t>756-a0f5883c-4d25-44f4-9a43-91c06b48019a</t>
-  </si>
-  <si>
-    <t>TAURO</t>
-  </si>
-  <si>
-    <t>2020-09-18</t>
-  </si>
-  <si>
-    <t>740.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 3036 - EDIF: TAURO R-101:CODIGO CLIENTE: 3036 - EDIF: TAURO</t>
-  </si>
-  <si>
-    <t>INV_906</t>
-  </si>
-  <si>
-    <t>752-394fe4cc-5a52-4faf-b598-037057c8a5bc</t>
-  </si>
-  <si>
-    <t>EMELEC</t>
-  </si>
-  <si>
-    <t>527.000 Bs.</t>
-  </si>
-  <si>
-    <t>R-100:CODIGO CLIENTE: 3129 - EDIF: EMELEC R-101:CODIGO CLIENTE: 3129 - EDIF: EMELEC</t>
-  </si>
-  <si>
-    <t>INV_844</t>
-  </si>
-  <si>
-    <t>743-7459ed28-b770-4c1b-85f4-aa9b572fdbc8</t>
-  </si>
-  <si>
-    <t>YAMASHIRO</t>
-  </si>
-  <si>
-    <t>R-100 /:Codigo Cliente: 2217 / Nombre del Edificio: YAMASHIRO R-101 /:Codigo Cliente: 2217 / Nombre del Edificio: YAMASHIRO</t>
-  </si>
-</sst>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">

</xml_diff>